<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@abb361de16290b49541051c004677e030db75528 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-ncpi-drs-file.xlsx
+++ b/StructureDefinition-ncpi-drs-file.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3042" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="533">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-25T15:36:07+00:00</t>
+    <t>2025-01-06T15:08:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1439,25 +1439,6 @@
   <si>
     <t xml:space="preserve">Attachment {https://nih-ncpi.github.io/ncpi-fhir-ig-2/StructureDefinition/ncpi-drs-attachment}
 </t>
-  </si>
-  <si>
-    <t>Content in a format defined elsewhere</t>
-  </si>
-  <si>
-    <t>For referring to data content defined in other formats.</t>
-  </si>
-  <si>
-    <t>When providing a summary view (for example with Observation.value[x]) Attachment should be represented with a brief display text such as "Signed Procedure Consent".</t>
-  </si>
-  <si>
-    <t>att-1:If the Attachment has data, it SHALL have a contentType {data.empty() or contentType.exists()}
-ele-1:All FHIR elements must have a @value or children unless an empty Parameters resource {hasValue() or (children().count() &gt; id.count()) or $this is Parameters}must-be-drs-uri:attachment.url must start with ^drs://. A drs:// hostname-based URI, as defined in the DRS documentation, that tells clients how to access this object. The intent of this field is to make DRS objects self-contained, and therefore easier for clients to store and pass around.  For example, if you arrive at this DRS JSON by resolving a compact identifier-based DRS URI, the `self_uri` presents you with a hostname and properly encoded DRS ID for use in subsequent `access` endpoint calls. {$this.url.matches('^drs://.*')}</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>ED/RP</t>
   </si>
   <si>
     <t>DocumentReference.content:DRS.attachment.id</t>
@@ -8719,20 +8700,18 @@
         <v>20</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="K55" t="s" s="2">
         <v>457</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>458</v>
+        <v>368</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>459</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>460</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
         <v>20</v>
@@ -8790,36 +8769,36 @@
         <v>93</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>461</v>
+        <v>105</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>20</v>
+        <v>370</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>462</v>
+        <v>362</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>20</v>
+        <v>371</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP55" t="s" s="2">
-        <v>463</v>
+        <v>372</v>
       </c>
       <c r="AQ55" t="s" s="2">
-        <v>20</v>
+        <v>373</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B56" t="s" s="2">
         <v>374</v>
@@ -8940,7 +8919,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B57" t="s" s="2">
         <v>375</v>
@@ -9063,7 +9042,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="B58" t="s" s="2">
         <v>377</v>
@@ -9186,7 +9165,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="B59" t="s" s="2">
         <v>387</v>
@@ -9309,7 +9288,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B60" t="s" s="2">
         <v>394</v>
@@ -9434,7 +9413,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B61" t="s" s="2">
         <v>403</v>
@@ -9559,7 +9538,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B62" t="s" s="2">
         <v>413</v>
@@ -9684,7 +9663,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B63" t="s" s="2">
         <v>421</v>
@@ -9809,7 +9788,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B64" t="s" s="2">
         <v>428</v>
@@ -9932,7 +9911,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B65" t="s" s="2">
         <v>435</v>
@@ -10055,7 +10034,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B66" t="s" s="2">
         <v>441</v>
@@ -10178,10 +10157,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -10207,13 +10186,13 @@
         <v>296</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -10263,7 +10242,7 @@
         <v>20</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>80</v>
@@ -10284,7 +10263,7 @@
         <v>20</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>20</v>
@@ -10301,10 +10280,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10422,10 +10401,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10545,10 +10524,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10670,10 +10649,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10696,13 +10675,13 @@
         <v>20</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -10753,7 +10732,7 @@
         <v>20</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>80</v>
@@ -10768,19 +10747,19 @@
         <v>105</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AO71" t="s" s="2">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="AP71" t="s" s="2">
         <v>20</v>
@@ -10791,10 +10770,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10820,13 +10799,13 @@
         <v>220</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="N72" t="s" s="2">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
@@ -10855,10 +10834,10 @@
         <v>238</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="Z72" t="s" s="2">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="AA72" t="s" s="2">
         <v>20</v>
@@ -10876,7 +10855,7 @@
         <v>20</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>80</v>
@@ -10894,10 +10873,10 @@
         <v>20</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>20</v>
@@ -10909,15 +10888,15 @@
         <v>20</v>
       </c>
       <c r="AQ72" t="s" s="2">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10940,13 +10919,13 @@
         <v>94</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -10997,7 +10976,7 @@
         <v>20</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>80</v>
@@ -11015,13 +10994,13 @@
         <v>20</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="AN73" t="s" s="2">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="AO73" t="s" s="2">
         <v>20</v>
@@ -11030,15 +11009,15 @@
         <v>20</v>
       </c>
       <c r="AQ73" t="s" s="2">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -11064,10 +11043,10 @@
         <v>220</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -11097,10 +11076,10 @@
         <v>238</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="Z74" t="s" s="2">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>20</v>
@@ -11118,7 +11097,7 @@
         <v>20</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>80</v>
@@ -11136,13 +11115,13 @@
         <v>20</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="AN74" t="s" s="2">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="AO74" t="s" s="2">
         <v>20</v>
@@ -11151,15 +11130,15 @@
         <v>20</v>
       </c>
       <c r="AQ74" t="s" s="2">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11185,16 +11164,16 @@
         <v>220</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="O75" t="s" s="2">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="P75" t="s" s="2">
         <v>20</v>
@@ -11222,10 +11201,10 @@
         <v>238</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="Z75" t="s" s="2">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="AA75" t="s" s="2">
         <v>20</v>
@@ -11243,7 +11222,7 @@
         <v>20</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>80</v>
@@ -11261,13 +11240,13 @@
         <v>20</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="AO75" t="s" s="2">
         <v>20</v>
@@ -11276,15 +11255,15 @@
         <v>20</v>
       </c>
       <c r="AQ75" t="s" s="2">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -11307,13 +11286,13 @@
         <v>20</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -11364,7 +11343,7 @@
         <v>20</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>80</v>
@@ -11397,15 +11376,15 @@
         <v>20</v>
       </c>
       <c r="AQ76" t="s" s="2">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11428,16 +11407,16 @@
         <v>20</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
@@ -11487,7 +11466,7 @@
         <v>20</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>80</v>
@@ -11505,13 +11484,13 @@
         <v>20</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="AO77" t="s" s="2">
         <v>20</v>
@@ -11520,7 +11499,7 @@
         <v>20</v>
       </c>
       <c r="AQ77" t="s" s="2">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@9fedbfbd981667bf017e0434fd9756f69abad73d 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-ncpi-drs-file.xlsx
+++ b/StructureDefinition-ncpi-drs-file.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-25T19:44:14+00:00</t>
+    <t>2025-06-27T14:40:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>81</v>

</xml_diff>